<commit_message>
enhance ABM models, expose corn ethanol process, and bump up version
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/LAOs/results/Stream tables.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/LAOs/results/Stream tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/733a0933307f0df0/Code/Bioindustrial-Park/BioSTEAM 2.x.x/biorefineries/LAOs/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D50878EB-B1F2-4580-AB5B-2CDB1F4FEC68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{D50878EB-B1F2-4580-AB5B-2CDB1F4FEC68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2B787ECA-FAD3-4525-B78E-FD8D99ADE6B3}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="960" windowWidth="17280" windowHeight="10044" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fermentation" sheetId="1" r:id="rId1"/>
@@ -1213,8 +1213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A21:P109"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="56" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="56" workbookViewId="0">
+      <selection activeCell="N73" sqref="N73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1443,7 +1443,7 @@
         <v>17.574962996697391</v>
       </c>
       <c r="C29" s="2">
-        <v>4398.4640604850247</v>
+        <v>4398.4640604850201</v>
       </c>
       <c r="D29" s="2">
         <v>3514.200843590148</v>
@@ -3466,7 +3466,7 @@
         <v>1.848541592234775</v>
       </c>
       <c r="C73" s="2">
-        <v>522.96848245247088</v>
+        <v>522.96848245247099</v>
       </c>
       <c r="D73" s="2">
         <v>369.62353845023648</v>
@@ -3499,7 +3499,7 @@
         <v>522.96847725506507</v>
       </c>
       <c r="N73" s="2">
-        <v>488.00733495530272</v>
+        <v>488.00733495530301</v>
       </c>
       <c r="O73" s="2">
         <v>488.00733495530272</v>
@@ -16564,7 +16564,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A62:AB150"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" workbookViewId="0">
+    <sheetView zoomScale="50" workbookViewId="0">
       <selection activeCell="H62" sqref="H62"/>
     </sheetView>
   </sheetViews>

</xml_diff>